<commit_message>
Stesura definitiva e presentazione
</commit_message>
<xml_diff>
--- a/Elaborato/Performance matrix determinant.xlsx
+++ b/Elaborato/Performance matrix determinant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\Tesi\Elaborato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F0959C-0E0A-40BC-A0EA-06B30A836A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4849B1-0C6F-4A32-AED2-10AC35982AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{13632D7E-4837-47AC-82B2-151CDE36C5FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{13632D7E-4837-47AC-82B2-151CDE36C5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>ELF</t>
   </si>
   <si>
-    <t>WASM</t>
-  </si>
-  <si>
     <t>NodeJS</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>NodeJS/ELF</t>
+  </si>
+  <si>
+    <t>WASI</t>
   </si>
 </sst>
 </file>
@@ -164,14 +164,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -187,8 +181,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -245,22 +242,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -331,26 +312,42 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -381,6 +378,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Tempo di</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> esecuzione</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -412,7 +439,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13850562147869527"/>
+          <c:y val="6.2526432943795229E-2"/>
+          <c:w val="0.83086027449648348"/>
+          <c:h val="0.76768297118119"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -454,6 +491,108 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6772226774820917E-2"/>
+                  <c:y val="2.3388937818498899E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1982166872757948E-2"/>
+                  <c:y val="-7.7741117084905286E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Foglio1!$B$3:$B$8</c:f>
@@ -521,7 +660,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>WASM</c:v>
+                  <c:v>WASI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -550,6 +689,174 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.6626553606283129E-2"/>
+                  <c:y val="-5.6744618108045507E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.4981309249416258E-2"/>
+                  <c:y val="-6.3422414435257368E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.2196390701705182E-2"/>
+                  <c:y val="-5.8970550217116016E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8476340362657794E-3"/>
+                  <c:y val="-5.5481795994198552E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.1972483250469216E-3"/>
+                  <c:y val="-7.7741117084906101E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Foglio1!$B$3:$B$8</c:f>
@@ -646,6 +953,152 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.6626553606283129E-2"/>
+                  <c:y val="-9.0133599744105522E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.4981309249416209E-2"/>
+                  <c:y val="-9.4585463962246791E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.4981309249416209E-2"/>
+                  <c:y val="-9.4585463962246707E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.4174711316879359E-3"/>
+                  <c:y val="-3.3222474903491822E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-5068-4ED5-895E-C012D81449BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Foglio1!$B$3:$B$8</c:f>
@@ -705,8 +1158,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -763,6 +1217,64 @@
                     <a:effectLst/>
                   </c:spPr>
                 </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="it-IT"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
                     <c:extLst>
@@ -847,6 +1359,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Lato della</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" baseline="0"/>
+                  <a:t> matrice</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -912,6 +1484,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Tempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1577,14 +2209,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
@@ -1615,14 +2247,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{026CF458-8DE2-4D81-8262-D72E1FBE1583}" name="Tabella1" displayName="Tabella1" ref="B2:G8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{026CF458-8DE2-4D81-8262-D72E1FBE1583}" name="Tabella1" displayName="Tabella1" ref="B2:G8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{320CEDAC-AD0A-4F21-8F36-A63CE703295A}" name=" " dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{56DF0C39-B99A-4007-AB21-389C9E6E654A}" name="ELF" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{DAE406FF-371E-487D-8EF3-82C23606D3BF}" name="WASM" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{2DF29553-BC54-4E28-9DE2-56129821E338}" name="NodeJS" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{320CEDAC-AD0A-4F21-8F36-A63CE703295A}" name=" " dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{56DF0C39-B99A-4007-AB21-389C9E6E654A}" name="ELF" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DAE406FF-371E-487D-8EF3-82C23606D3BF}" name="WASI" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2DF29553-BC54-4E28-9DE2-56129821E338}" name="NodeJS" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{2684886E-A0DD-4AFA-9E35-DFFE4540F11F}" name="WASM/ELF" dataDxfId="1">
-      <calculatedColumnFormula>Tabella1[[#This Row],[WASM]]/Tabella1[[#This Row],[ELF]]</calculatedColumnFormula>
+      <calculatedColumnFormula>Tabella1[[#This Row],[WASI]]/Tabella1[[#This Row],[ELF]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{2028D11C-FE3D-42A9-94DE-B5C1F7315532}" name="NodeJS/ELF" dataDxfId="0">
       <calculatedColumnFormula>Tabella1[[#This Row],[NodeJS]]/Tabella1[[#This Row],[ELF]]</calculatedColumnFormula>
@@ -1931,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D60F807-38FA-4AD4-80AB-3D13ADFD741E}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,164 +2575,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
         <v>100</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>1E-3</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>0.40200000000000002</v>
       </c>
-      <c r="F3" s="3">
-        <f>Tabella1[[#This Row],[WASM]]/Tabella1[[#This Row],[ELF]]</f>
+      <c r="F3" s="1">
+        <f>Tabella1[[#This Row],[WASI]]/Tabella1[[#This Row],[ELF]]</f>
         <v>67</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="1">
         <f>Tabella1[[#This Row],[NodeJS]]/Tabella1[[#This Row],[ELF]]</f>
         <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1">
         <v>1000</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>0.27500000000000002</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>0.33800000000000002</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>0.92200000000000004</v>
       </c>
-      <c r="F4" s="3">
-        <f>Tabella1[[#This Row],[WASM]]/Tabella1[[#This Row],[ELF]]</f>
+      <c r="F4" s="1">
+        <f>Tabella1[[#This Row],[WASI]]/Tabella1[[#This Row],[ELF]]</f>
         <v>1.229090909090909</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="1">
         <f>Tabella1[[#This Row],[NodeJS]]/Tabella1[[#This Row],[ELF]]</f>
         <v>3.3527272727272726</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="1">
         <v>2000</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>2.3239999999999998</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>3.3690000000000002</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>7.1859999999999999</v>
       </c>
-      <c r="F5" s="3">
-        <f>Tabella1[[#This Row],[WASM]]/Tabella1[[#This Row],[ELF]]</f>
+      <c r="F5" s="1">
+        <f>Tabella1[[#This Row],[WASI]]/Tabella1[[#This Row],[ELF]]</f>
         <v>1.4496557659208265</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="1">
         <f>Tabella1[[#This Row],[NodeJS]]/Tabella1[[#This Row],[ELF]]</f>
         <v>3.092082616179002</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="1">
         <v>5000</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>44.728000000000002</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>52.372</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>105.41800000000001</v>
       </c>
-      <c r="F6" s="3">
-        <f>Tabella1[[#This Row],[WASM]]/Tabella1[[#This Row],[ELF]]</f>
+      <c r="F6" s="1">
+        <f>Tabella1[[#This Row],[WASI]]/Tabella1[[#This Row],[ELF]]</f>
         <v>1.1708996601681274</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="1">
         <f>Tabella1[[#This Row],[NodeJS]]/Tabella1[[#This Row],[ELF]]</f>
         <v>2.3568681810051868</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="1">
         <v>10000</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>325.39600000000002</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>381.04500000000002</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>818.37</v>
       </c>
-      <c r="F7" s="3">
-        <f>Tabella1[[#This Row],[WASM]]/Tabella1[[#This Row],[ELF]]</f>
+      <c r="F7" s="1">
+        <f>Tabella1[[#This Row],[WASI]]/Tabella1[[#This Row],[ELF]]</f>
         <v>1.1710193118538643</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="1">
         <f>Tabella1[[#This Row],[NodeJS]]/Tabella1[[#This Row],[ELF]]</f>
         <v>2.5149971112121845</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>20000</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8" t="e">
-        <f>Tabella1[[#This Row],[WASM]]/Tabella1[[#This Row],[ELF]]</f>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4" t="e">
+        <f>Tabella1[[#This Row],[WASI]]/Tabella1[[#This Row],[ELF]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="8" t="e">
+      <c r="G8" s="4" t="e">
         <f>Tabella1[[#This Row],[NodeJS]]/Tabella1[[#This Row],[ELF]]</f>
         <v>#DIV/0!</v>
       </c>

</xml_diff>